<commit_message>
Residential rates version to br checked
</commit_message>
<xml_diff>
--- a/PG&E residential .xlsx
+++ b/PG&E residential .xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hectortavera/workspace/Rate_Desing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2C7397E-AABA-9947-83E8-5DF5EC5B5C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F7E46C-63DC-1D4E-944F-9CB873D4ACB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30960" yWindow="-520" windowWidth="25460" windowHeight="17140" xr2:uid="{6EA4E839-D09B-E447-B34D-B7C5197156AC}"/>
+    <workbookView xWindow="28880" yWindow="-520" windowWidth="19960" windowHeight="18900" xr2:uid="{6EA4E839-D09B-E447-B34D-B7C5197156AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Residential Rates " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="109">
   <si>
     <t>Rate Desing structure for GridLAB-D</t>
   </si>
@@ -524,9 +524,6 @@
     <t xml:space="preserve">Location must be given to select territory </t>
   </si>
   <si>
-    <t>Monthly baseline usage in summer = Tier 1 daily usage x billing days in a month (usually 30 for calculations)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Usage must be obtained in kWh for conversion </t>
   </si>
   <si>
@@ -542,41 +539,120 @@
     <t xml:space="preserve">Transmission </t>
   </si>
   <si>
-    <t xml:space="preserve">Public Purpose Porgrams </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nuclear Decommissioning </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Responsibility surcharge </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy cost recovery </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DWR Bond </t>
-  </si>
-  <si>
-    <t>Competition Transition Charges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power Charge Indiference Adjust </t>
-  </si>
-  <si>
     <t xml:space="preserve">% Rate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly baseline usage in summer = Tier 1 daily usage x billing days in a month </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmission Rate Adjustment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliability Services </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public Purpose Programs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuclear Decomissioning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Competition Transition Charges </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Cost Recovery Amount </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildfire Fund Charge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">New System Generation Charge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">101% - 400% of Baseline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; 400% of Baseline </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate </t>
+  </si>
+  <si>
+    <t>Bill Components for Direct Access or CCA Customer</t>
+  </si>
+  <si>
+    <t>Conservation Incentive Adjustment IOU</t>
+  </si>
+  <si>
+    <t>Conservation Incentive Adjustment DA/CCA</t>
+  </si>
+  <si>
+    <t>CTC Charge per kWh</t>
+  </si>
+  <si>
+    <t>Energy Cost Recovery Amount per kWh</t>
+  </si>
+  <si>
+    <t>Wildfire Fund Charge per kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Charge Indiference Adjustment per kWh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019 Vintage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020 Vintage </t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="166" formatCode="00.0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="&quot;  &quot;0.0"/>
+    <numFmt numFmtId="182" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -779,7 +855,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,6 +877,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,7 +1036,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -962,15 +1050,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -978,21 +1062,12 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1019,18 +1094,12 @@
     </xf>
     <xf numFmtId="7" fontId="20" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1119,15 +1188,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1444,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1B52A0-0F9F-F84F-8944-68FF03780A4D}">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80:F84"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1455,7 +1563,7 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.1640625" customWidth="1"/>
@@ -1535,91 +1643,91 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22" t="s">
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="15" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="17" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="24"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="24">
         <v>0.32854</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="24">
         <v>0.24373</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="24">
         <v>0.30671999999999999</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="24">
         <v>0.38340000000000002</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="26">
         <v>-0.34861999999999999</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="27">
         <v>-17.86</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="25">
         <v>0.26249</v>
       </c>
     </row>
@@ -1640,19 +1748,19 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="5"/>
@@ -1661,7 +1769,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="75" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="9">
@@ -1674,7 +1782,7 @@
         <f>F8</f>
         <v>0.24373</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="1"/>
@@ -1685,7 +1793,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="75" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="9">
@@ -1698,7 +1806,7 @@
         <f>G8</f>
         <v>0.30671999999999999</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="1"/>
@@ -1709,7 +1817,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="75" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="9">
@@ -1722,7 +1830,7 @@
         <f>H8</f>
         <v>0.38340000000000002</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="1"/>
@@ -1745,10 +1853,10 @@
     <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="6">
         <f>C8</f>
         <v>0.32854</v>
@@ -1776,18 +1884,18 @@
     <row r="17" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="14">
+      <c r="D17" s="71"/>
+      <c r="E17" s="13">
         <f>J8</f>
         <v>-17.86</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="72"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1808,781 +1916,781 @@
     </row>
     <row r="19" spans="1:11" ht="22" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="33" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="33" t="s">
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
     </row>
     <row r="20" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="37" t="s">
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="66"/>
     </row>
     <row r="21" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41" t="s">
+      <c r="E21" s="33"/>
+      <c r="F21" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="39" t="s">
+      <c r="G21" s="35"/>
+      <c r="H21" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41" t="s">
+      <c r="J21" s="33"/>
+      <c r="K21" s="34" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44" t="s">
+      <c r="C22" s="36"/>
+      <c r="D22" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46" t="s">
+      <c r="E22" s="38"/>
+      <c r="F22" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="42"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="44" t="s">
+      <c r="G22" s="35"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="45"/>
-      <c r="K22" s="46" t="s">
+      <c r="J22" s="38"/>
+      <c r="K22" s="39" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="46"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="39"/>
     </row>
     <row r="24" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="48" t="s">
+      <c r="D24" s="42"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I24" s="46"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="46"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="39"/>
     </row>
     <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="51"/>
-      <c r="F25" s="50" t="s">
+      <c r="E25" s="44"/>
+      <c r="F25" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="50" t="s">
+      <c r="G25" s="35"/>
+      <c r="H25" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="50" t="s">
+      <c r="I25" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="J25" s="51"/>
-      <c r="K25" s="50" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="43" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="47" t="s">
+      <c r="C26" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="52">
+      <c r="D26" s="45">
         <v>27.4</v>
       </c>
-      <c r="E26" s="53"/>
-      <c r="F26" s="52">
+      <c r="E26" s="46"/>
+      <c r="F26" s="45">
         <v>14.7</v>
       </c>
-      <c r="G26" s="42"/>
-      <c r="H26" s="47" t="s">
+      <c r="G26" s="35"/>
+      <c r="H26" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="54">
+      <c r="I26" s="47">
         <v>16</v>
       </c>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46">
+      <c r="J26" s="39"/>
+      <c r="K26" s="39">
         <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="52">
+      <c r="D27" s="45">
         <v>27.4</v>
       </c>
-      <c r="E27" s="53"/>
-      <c r="F27" s="52">
+      <c r="E27" s="46"/>
+      <c r="F27" s="45">
         <v>14.7</v>
       </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="47" t="s">
+      <c r="G27" s="35"/>
+      <c r="H27" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="54">
+      <c r="I27" s="47">
         <v>8.9</v>
       </c>
-      <c r="J27" s="46"/>
-      <c r="K27" s="46">
+      <c r="J27" s="39"/>
+      <c r="K27" s="39">
         <v>7.3</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="52">
+      <c r="D28" s="45">
         <v>28.1</v>
       </c>
-      <c r="E28" s="53"/>
-      <c r="F28" s="52">
+      <c r="E28" s="46"/>
+      <c r="F28" s="45">
         <v>13.6</v>
       </c>
-      <c r="G28" s="42"/>
-      <c r="H28" s="47" t="s">
+      <c r="G28" s="35"/>
+      <c r="H28" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I28" s="54">
+      <c r="I28" s="47">
         <v>20.9</v>
       </c>
-      <c r="J28" s="46"/>
-      <c r="K28" s="46">
+      <c r="J28" s="39"/>
+      <c r="K28" s="39">
         <v>9.6</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="52">
+      <c r="D29" s="45">
         <v>24.9</v>
       </c>
-      <c r="E29" s="53"/>
-      <c r="F29" s="52">
+      <c r="E29" s="46"/>
+      <c r="F29" s="45">
         <v>13.1</v>
       </c>
-      <c r="G29" s="42"/>
-      <c r="H29" s="47" t="s">
+      <c r="G29" s="35"/>
+      <c r="H29" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="I29" s="54">
+      <c r="I29" s="47">
         <v>18.7</v>
       </c>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46">
+      <c r="J29" s="39"/>
+      <c r="K29" s="39">
         <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="52">
+      <c r="D30" s="45">
         <v>13.6</v>
       </c>
-      <c r="E30" s="53"/>
-      <c r="F30" s="54">
+      <c r="E30" s="46"/>
+      <c r="F30" s="47">
         <v>9</v>
       </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="47" t="s">
+      <c r="G30" s="35"/>
+      <c r="H30" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="54">
+      <c r="I30" s="47">
         <v>7.5</v>
       </c>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46">
+      <c r="J30" s="39"/>
+      <c r="K30" s="39">
         <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="52">
+      <c r="D31" s="45">
         <v>16.899999999999999</v>
       </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="52">
+      <c r="E31" s="46"/>
+      <c r="F31" s="45">
         <v>11.2</v>
       </c>
-      <c r="G31" s="42"/>
-      <c r="H31" s="47" t="s">
+      <c r="G31" s="35"/>
+      <c r="H31" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="54">
+      <c r="I31" s="47">
         <v>10.9</v>
       </c>
-      <c r="J31" s="46"/>
-      <c r="K31" s="54">
+      <c r="J31" s="39"/>
+      <c r="K31" s="47">
         <v>6.3</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="52">
+      <c r="D32" s="45">
         <v>20</v>
       </c>
-      <c r="E32" s="53"/>
-      <c r="F32" s="52">
+      <c r="E32" s="46"/>
+      <c r="F32" s="45">
         <v>11.8</v>
       </c>
-      <c r="G32" s="42"/>
-      <c r="H32" s="47" t="s">
+      <c r="G32" s="35"/>
+      <c r="H32" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="I32" s="54">
+      <c r="I32" s="47">
         <v>23.6</v>
       </c>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46">
+      <c r="J32" s="39"/>
+      <c r="K32" s="39">
         <v>11.7</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="52">
+      <c r="D33" s="45">
         <v>15.4</v>
       </c>
-      <c r="E33" s="53"/>
-      <c r="F33" s="52">
+      <c r="E33" s="46"/>
+      <c r="F33" s="45">
         <v>12.9</v>
       </c>
-      <c r="G33" s="42"/>
-      <c r="H33" s="47" t="s">
+      <c r="G33" s="35"/>
+      <c r="H33" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I33" s="54">
+      <c r="I33" s="47">
         <v>8.9</v>
       </c>
-      <c r="J33" s="46"/>
-      <c r="K33" s="54">
+      <c r="J33" s="39"/>
+      <c r="K33" s="47">
         <v>7.3</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="52">
+      <c r="D34" s="45">
         <v>25.3</v>
       </c>
-      <c r="E34" s="53"/>
-      <c r="F34" s="52">
+      <c r="E34" s="46"/>
+      <c r="F34" s="45">
         <v>14.4</v>
       </c>
-      <c r="G34" s="42"/>
-      <c r="H34" s="47" t="s">
+      <c r="G34" s="35"/>
+      <c r="H34" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I34" s="54">
+      <c r="I34" s="47">
         <v>12.6</v>
       </c>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46">
+      <c r="J34" s="39"/>
+      <c r="K34" s="39">
         <v>7.1</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="56">
+      <c r="D35" s="49">
         <v>16.5</v>
       </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="57">
+      <c r="E35" s="44"/>
+      <c r="F35" s="50">
         <v>9.4</v>
       </c>
-      <c r="G35" s="42"/>
-      <c r="H35" s="55" t="s">
+      <c r="G35" s="35"/>
+      <c r="H35" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="I35" s="57">
+      <c r="I35" s="50">
         <v>7</v>
       </c>
-      <c r="J35" s="50"/>
-      <c r="K35" s="57">
+      <c r="J35" s="43"/>
+      <c r="K35" s="50">
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="54"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="47"/>
     </row>
     <row r="37" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="47" t="s">
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="I37" s="58"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
     </row>
     <row r="38" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="50" t="s">
+      <c r="D38" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="51"/>
-      <c r="F38" s="50" t="s">
+      <c r="E38" s="44"/>
+      <c r="F38" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="42"/>
-      <c r="H38" s="50" t="s">
+      <c r="G38" s="35"/>
+      <c r="H38" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="I38" s="50" t="s">
+      <c r="I38" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="J38" s="51"/>
-      <c r="K38" s="50" t="s">
+      <c r="J38" s="44"/>
+      <c r="K38" s="43" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="47" t="s">
+      <c r="C39" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="52">
+      <c r="D39" s="45">
         <v>12</v>
       </c>
-      <c r="E39" s="46"/>
-      <c r="F39" s="54">
+      <c r="E39" s="39"/>
+      <c r="F39" s="47">
         <v>5.2</v>
       </c>
-      <c r="G39" s="42"/>
-      <c r="H39" s="47" t="s">
+      <c r="G39" s="35"/>
+      <c r="H39" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="I39" s="52">
+      <c r="I39" s="45">
         <v>14.2</v>
       </c>
-      <c r="J39" s="46"/>
-      <c r="K39" s="59">
+      <c r="J39" s="39"/>
+      <c r="K39" s="52">
         <v>4.8</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="47" t="s">
+      <c r="C40" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="54">
+      <c r="D40" s="47">
         <v>12</v>
       </c>
-      <c r="E40" s="46"/>
-      <c r="F40" s="54">
+      <c r="E40" s="39"/>
+      <c r="F40" s="47">
         <v>5.2</v>
       </c>
-      <c r="G40" s="42"/>
-      <c r="H40" s="47" t="s">
+      <c r="G40" s="35"/>
+      <c r="H40" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="I40" s="54">
+      <c r="I40" s="47">
         <v>10.3</v>
       </c>
-      <c r="J40" s="46"/>
-      <c r="K40" s="59">
+      <c r="J40" s="39"/>
+      <c r="K40" s="52">
         <v>5.4</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="52">
+      <c r="D41" s="45">
         <v>11.3</v>
       </c>
-      <c r="E41" s="46"/>
-      <c r="F41" s="54">
+      <c r="E41" s="39"/>
+      <c r="F41" s="47">
         <v>5.2</v>
       </c>
-      <c r="G41" s="42"/>
-      <c r="H41" s="47" t="s">
+      <c r="G41" s="35"/>
+      <c r="H41" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="54">
+      <c r="I41" s="47">
         <v>18.600000000000001</v>
       </c>
-      <c r="J41" s="46"/>
-      <c r="K41" s="59">
+      <c r="J41" s="39"/>
+      <c r="K41" s="52">
         <v>7.9</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="47" t="s">
+      <c r="C42" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="52">
+      <c r="D42" s="45">
         <v>11.1</v>
       </c>
-      <c r="E42" s="46"/>
-      <c r="F42" s="54">
+      <c r="E42" s="39"/>
+      <c r="F42" s="47">
         <v>5.2</v>
       </c>
-      <c r="G42" s="42"/>
-      <c r="H42" s="47" t="s">
+      <c r="G42" s="35"/>
+      <c r="H42" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="54">
+      <c r="I42" s="47">
         <v>15.8</v>
       </c>
-      <c r="J42" s="46"/>
-      <c r="K42" s="59">
+      <c r="J42" s="39"/>
+      <c r="K42" s="52">
         <v>6.7</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="47" t="s">
+      <c r="C43" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="54">
+      <c r="D43" s="47">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E43" s="46"/>
-      <c r="F43" s="54">
+      <c r="E43" s="39"/>
+      <c r="F43" s="47">
         <v>4.5</v>
       </c>
-      <c r="G43" s="42"/>
-      <c r="H43" s="47" t="s">
+      <c r="G43" s="35"/>
+      <c r="H43" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="I43" s="54">
+      <c r="I43" s="47">
         <v>6.8</v>
       </c>
-      <c r="J43" s="46"/>
-      <c r="K43" s="59">
+      <c r="J43" s="39"/>
+      <c r="K43" s="52">
         <v>3.8</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="47" t="s">
+      <c r="C44" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="54">
+      <c r="D44" s="47">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E44" s="46"/>
-      <c r="F44" s="54">
+      <c r="E44" s="39"/>
+      <c r="F44" s="47">
         <v>5</v>
       </c>
-      <c r="G44" s="42"/>
-      <c r="H44" s="47" t="s">
+      <c r="G44" s="35"/>
+      <c r="H44" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="54">
+      <c r="I44" s="47">
         <v>7.5</v>
       </c>
-      <c r="J44" s="46"/>
-      <c r="K44" s="59">
+      <c r="J44" s="39"/>
+      <c r="K44" s="52">
         <v>4.2</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="47" t="s">
+      <c r="C45" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D45" s="52">
+      <c r="D45" s="45">
         <v>10.7</v>
       </c>
-      <c r="E45" s="46"/>
-      <c r="F45" s="54">
+      <c r="E45" s="39"/>
+      <c r="F45" s="47">
         <v>5.3</v>
       </c>
-      <c r="G45" s="42"/>
-      <c r="H45" s="47" t="s">
+      <c r="G45" s="35"/>
+      <c r="H45" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="I45" s="54">
+      <c r="I45" s="47">
         <v>20.2</v>
       </c>
-      <c r="J45" s="46"/>
-      <c r="K45" s="59">
+      <c r="J45" s="39"/>
+      <c r="K45" s="52">
         <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="47" t="s">
+      <c r="C46" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="52">
+      <c r="D46" s="45">
         <v>10.5</v>
       </c>
-      <c r="E46" s="46"/>
-      <c r="F46" s="54">
+      <c r="E46" s="39"/>
+      <c r="F46" s="47">
         <v>5.9</v>
       </c>
-      <c r="G46" s="42"/>
-      <c r="H46" s="47" t="s">
+      <c r="G46" s="35"/>
+      <c r="H46" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I46" s="54">
+      <c r="I46" s="47">
         <v>10.3</v>
       </c>
-      <c r="J46" s="46"/>
-      <c r="K46" s="59">
+      <c r="J46" s="39"/>
+      <c r="K46" s="52">
         <v>5.4</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="47" t="s">
+      <c r="C47" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="52">
+      <c r="D47" s="45">
         <v>12.1</v>
       </c>
-      <c r="E47" s="46"/>
-      <c r="F47" s="54">
+      <c r="E47" s="39"/>
+      <c r="F47" s="47">
         <v>8.3000000000000007</v>
       </c>
-      <c r="G47" s="42"/>
-      <c r="H47" s="47" t="s">
+      <c r="G47" s="35"/>
+      <c r="H47" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="I47" s="54">
+      <c r="I47" s="47">
         <v>11</v>
       </c>
-      <c r="J47" s="46"/>
-      <c r="K47" s="59">
+      <c r="J47" s="39"/>
+      <c r="K47" s="52">
         <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="55" t="s">
+      <c r="C48" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="57">
+      <c r="D48" s="50">
         <v>8.1</v>
       </c>
-      <c r="E48" s="50"/>
-      <c r="F48" s="57">
+      <c r="E48" s="43"/>
+      <c r="F48" s="50">
         <v>5.6</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="55" t="s">
+      <c r="G48" s="35"/>
+      <c r="H48" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="I48" s="57">
+      <c r="I48" s="50">
         <v>6.2</v>
       </c>
-      <c r="J48" s="50"/>
-      <c r="K48" s="60">
+      <c r="J48" s="43"/>
+      <c r="K48" s="53">
         <v>4.5</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="63"/>
-      <c r="K49" s="64"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="55"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="57"/>
     </row>
     <row r="50" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="65" t="s">
+      <c r="C50" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="62"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="62"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="62"/>
-      <c r="J50" s="63"/>
-      <c r="K50" s="64"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="57"/>
     </row>
     <row r="51" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="42"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
     </row>
     <row r="52" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="D52" s="42"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
-      <c r="C53" s="67" t="s">
+      <c r="C53" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="68" t="s">
+      <c r="C54" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="42"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
@@ -2613,17 +2721,17 @@
     <row r="57" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
-      <c r="D57" s="70" t="s">
+      <c r="D57" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="69" t="s">
+      <c r="E57" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69" t="s">
+      <c r="F57" s="67"/>
+      <c r="G57" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H57" s="69"/>
+      <c r="H57" s="67"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
@@ -2632,19 +2740,19 @@
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
-      <c r="D58" s="70" t="s">
+      <c r="D58" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="70" t="s">
+      <c r="E58" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="F58" s="70" t="s">
+      <c r="F58" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="G58" s="70" t="s">
+      <c r="G58" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="H58" s="70" t="s">
+      <c r="H58" s="62" t="s">
         <v>28</v>
       </c>
       <c r="I58" s="5"/>
@@ -2655,10 +2763,10 @@
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
-      <c r="D59" s="70" t="s">
+      <c r="D59" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="E59" s="73" t="s">
+      <c r="E59" s="65" t="s">
         <v>20</v>
       </c>
       <c r="F59" s="8" t="s">
@@ -2678,22 +2786,22 @@
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
-      <c r="D60" s="71" t="s">
+      <c r="D60" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="E60" s="73">
+      <c r="E60" s="65">
         <f>I39</f>
         <v>14.2</v>
       </c>
-      <c r="F60" s="73">
+      <c r="F60" s="65">
         <f>D39</f>
         <v>12</v>
       </c>
-      <c r="G60" s="73">
+      <c r="G60" s="65">
         <f>I26</f>
         <v>16</v>
       </c>
-      <c r="H60" s="72">
+      <c r="H60" s="64">
         <f>D26</f>
         <v>27.4</v>
       </c>
@@ -2705,22 +2813,22 @@
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
-      <c r="D61" s="71" t="s">
+      <c r="D61" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="E61" s="73">
+      <c r="E61" s="65">
         <f t="shared" ref="E61:E69" si="0">I40</f>
         <v>10.3</v>
       </c>
-      <c r="F61" s="73">
+      <c r="F61" s="65">
         <f t="shared" ref="F61:F69" si="1">D40</f>
         <v>12</v>
       </c>
-      <c r="G61" s="73">
+      <c r="G61" s="65">
         <f t="shared" ref="G61:G69" si="2">I27</f>
         <v>8.9</v>
       </c>
-      <c r="H61" s="72">
+      <c r="H61" s="64">
         <f t="shared" ref="H61:H69" si="3">D27</f>
         <v>27.4</v>
       </c>
@@ -2732,22 +2840,22 @@
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
-      <c r="D62" s="71" t="s">
+      <c r="D62" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="73">
+      <c r="E62" s="65">
         <f t="shared" si="0"/>
         <v>18.600000000000001</v>
       </c>
-      <c r="F62" s="73">
+      <c r="F62" s="65">
         <f t="shared" si="1"/>
         <v>11.3</v>
       </c>
-      <c r="G62" s="73">
+      <c r="G62" s="65">
         <f t="shared" si="2"/>
         <v>20.9</v>
       </c>
-      <c r="H62" s="72">
+      <c r="H62" s="64">
         <f t="shared" si="3"/>
         <v>28.1</v>
       </c>
@@ -2759,22 +2867,22 @@
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
-      <c r="D63" s="71" t="s">
+      <c r="D63" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="E63" s="73">
+      <c r="E63" s="65">
         <f t="shared" si="0"/>
         <v>15.8</v>
       </c>
-      <c r="F63" s="73">
+      <c r="F63" s="65">
         <f t="shared" si="1"/>
         <v>11.1</v>
       </c>
-      <c r="G63" s="73">
+      <c r="G63" s="65">
         <f t="shared" si="2"/>
         <v>18.7</v>
       </c>
-      <c r="H63" s="72">
+      <c r="H63" s="64">
         <f t="shared" si="3"/>
         <v>24.9</v>
       </c>
@@ -2786,22 +2894,22 @@
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
-      <c r="D64" s="71" t="s">
+      <c r="D64" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="E64" s="73">
+      <c r="E64" s="65">
         <f t="shared" si="0"/>
         <v>6.8</v>
       </c>
-      <c r="F64" s="73">
+      <c r="F64" s="65">
         <f t="shared" si="1"/>
         <v>8.1999999999999993</v>
       </c>
-      <c r="G64" s="73">
+      <c r="G64" s="65">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
-      <c r="H64" s="72">
+      <c r="H64" s="64">
         <f t="shared" si="3"/>
         <v>13.6</v>
       </c>
@@ -2813,22 +2921,22 @@
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
-      <c r="D65" s="71" t="s">
+      <c r="D65" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="E65" s="73">
+      <c r="E65" s="65">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F65" s="73">
+      <c r="F65" s="65">
         <f t="shared" si="1"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="G65" s="73">
+      <c r="G65" s="65">
         <f t="shared" si="2"/>
         <v>10.9</v>
       </c>
-      <c r="H65" s="72">
+      <c r="H65" s="64">
         <f t="shared" si="3"/>
         <v>16.899999999999999</v>
       </c>
@@ -2837,85 +2945,85 @@
       <c r="K65" s="5"/>
     </row>
     <row r="66" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="D66" s="71" t="s">
+      <c r="D66" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="E66" s="73">
+      <c r="E66" s="65">
         <f t="shared" si="0"/>
         <v>20.2</v>
       </c>
-      <c r="F66" s="73">
+      <c r="F66" s="65">
         <f t="shared" si="1"/>
         <v>10.7</v>
       </c>
-      <c r="G66" s="73">
+      <c r="G66" s="65">
         <f t="shared" si="2"/>
         <v>23.6</v>
       </c>
-      <c r="H66" s="72">
+      <c r="H66" s="64">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="D67" s="71" t="s">
+      <c r="D67" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="E67" s="73">
+      <c r="E67" s="65">
         <f t="shared" si="0"/>
         <v>10.3</v>
       </c>
-      <c r="F67" s="73">
+      <c r="F67" s="65">
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
-      <c r="G67" s="73">
+      <c r="G67" s="65">
         <f t="shared" si="2"/>
         <v>8.9</v>
       </c>
-      <c r="H67" s="72">
+      <c r="H67" s="64">
         <f t="shared" si="3"/>
         <v>15.4</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="D68" s="71" t="s">
+      <c r="D68" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="E68" s="73">
+      <c r="E68" s="65">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F68" s="73">
+      <c r="F68" s="65">
         <f t="shared" si="1"/>
         <v>12.1</v>
       </c>
-      <c r="G68" s="73">
+      <c r="G68" s="65">
         <f t="shared" si="2"/>
         <v>12.6</v>
       </c>
-      <c r="H68" s="72">
+      <c r="H68" s="64">
         <f t="shared" si="3"/>
         <v>25.3</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="D69" s="71" t="s">
+      <c r="D69" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E69" s="73">
+      <c r="E69" s="65">
         <f t="shared" si="0"/>
         <v>6.2</v>
       </c>
-      <c r="F69" s="73">
+      <c r="F69" s="65">
         <f t="shared" si="1"/>
         <v>8.1</v>
       </c>
-      <c r="G69" s="73">
+      <c r="G69" s="65">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="H69" s="72">
+      <c r="H69" s="64">
         <f t="shared" si="3"/>
         <v>16.5</v>
       </c>
@@ -2951,7 +3059,7 @@
     </row>
     <row r="74" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="D74" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -2965,80 +3073,552 @@
     </row>
     <row r="76" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
     <row r="78" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="C78" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="C78" s="81" t="s">
+        <v>71</v>
+      </c>
+      <c r="D78" s="81"/>
     </row>
     <row r="79" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="C79" s="2"/>
-      <c r="F79" t="s">
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="79" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="D80" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="E80" s="80">
+        <v>0.11738</v>
+      </c>
+      <c r="F80" s="78">
+        <f>E80/$E$92</f>
+        <v>0.41612308564946116</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D81" s="79" t="s">
+        <v>73</v>
+      </c>
+      <c r="E81" s="80">
+        <v>9.9779999999999994E-2</v>
+      </c>
+      <c r="F81" s="78">
+        <f t="shared" ref="F81:F90" si="4">E81/$E$92</f>
+        <v>0.35372943845717525</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D82" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E82" s="80">
+        <v>3.5950000000000003E-2</v>
+      </c>
+      <c r="F82" s="78">
+        <f t="shared" si="4"/>
+        <v>0.12744611457742486</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D83" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="E83" s="80">
+        <v>3.14E-3</v>
+      </c>
+      <c r="F83" s="78">
+        <f t="shared" si="4"/>
+        <v>1.1131593874078275E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D84" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="E84" s="80">
+        <v>-6.6E-4</v>
+      </c>
+      <c r="F84" s="78">
+        <f t="shared" si="4"/>
+        <v>-2.3397617697107202E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D85" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E85" s="80">
+        <v>1.2959999999999999E-2</v>
+      </c>
+      <c r="F85" s="78">
+        <f t="shared" si="4"/>
+        <v>4.5944412932501413E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D86" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="E86" s="80">
+        <v>1.01E-3</v>
+      </c>
+      <c r="F86" s="78">
+        <f t="shared" si="4"/>
+        <v>3.5805445263754963E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D87" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" s="80">
+        <v>9.6000000000000002E-4</v>
+      </c>
+      <c r="F87" s="78">
+        <f t="shared" si="4"/>
+        <v>3.4032898468519569E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D88" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="E88" s="80">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="F88" s="78">
+        <f t="shared" si="4"/>
+        <v>1.7725467952353944E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D89" s="79" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D80" t="s">
+      <c r="E89" s="80">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="F89" s="78">
+        <f t="shared" si="4"/>
+        <v>2.0561542824730571E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D90" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="E90" s="80">
+        <v>5.7099999999999998E-3</v>
+      </c>
+      <c r="F90" s="78">
+        <f t="shared" si="4"/>
+        <v>2.0242484401588202E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="3:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="D92" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="E92" s="77">
+        <f>SUM(E80:E90)</f>
+        <v>0.28208</v>
+      </c>
+      <c r="F92" s="78">
+        <f>SUM(F80:F90)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+    </row>
+    <row r="94" spans="3:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="C94" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="D94" s="81"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D95" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="80">
+        <v>-3.7780000000000001E-2</v>
+      </c>
+      <c r="F95" s="6">
+        <f>$E$92+E95</f>
+        <v>0.24429999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D96" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E96" s="80">
+        <v>2.5350000000000001E-2</v>
+      </c>
+      <c r="F96" s="6">
+        <f t="shared" ref="F96:F97" si="5">$E$92+E96</f>
+        <v>0.30742999999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D97" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" s="80">
+        <v>0.1022</v>
+      </c>
+      <c r="F97" s="6">
+        <f t="shared" si="5"/>
+        <v>0.38428000000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="3:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="C99" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="D99" s="81"/>
+      <c r="E99" s="81"/>
+    </row>
+    <row r="100" spans="3:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="C100" s="2"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="G100" s="79" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D101" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="E101" s="80"/>
+      <c r="F101" s="82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D102" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="F80" s="74"/>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D81" t="s">
+      <c r="E102" s="80"/>
+      <c r="F102" s="80">
+        <f>E81</f>
+        <v>9.9779999999999994E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D103" s="79" t="s">
         <v>74</v>
       </c>
-      <c r="F81" s="74"/>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D82" t="s">
-        <v>75</v>
-      </c>
-      <c r="F82" s="74"/>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
-        <v>76</v>
-      </c>
-      <c r="F83" s="74"/>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+      <c r="E103" s="80"/>
+      <c r="F103" s="80">
+        <f t="shared" ref="F103:F111" si="6">E82</f>
+        <v>3.5950000000000003E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D104" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="F84" s="74"/>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
+      <c r="E104" s="80"/>
+      <c r="F104" s="80">
+        <f t="shared" si="6"/>
+        <v>3.14E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D105" s="79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D86" t="s">
+      <c r="E105" s="80"/>
+      <c r="F105" s="80">
+        <f t="shared" si="6"/>
+        <v>-6.6E-4</v>
+      </c>
+    </row>
+    <row r="106" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D106" s="79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D87" t="s">
+      <c r="E106" s="80"/>
+      <c r="F106" s="80">
+        <f t="shared" si="6"/>
+        <v>1.2959999999999999E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D107" s="79" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D88" t="s">
+      <c r="E107" s="80"/>
+      <c r="F107" s="80">
+        <f t="shared" si="6"/>
+        <v>1.01E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D108" s="79" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D89" t="s">
-        <v>82</v>
+      <c r="E108" s="80"/>
+      <c r="F108" s="80">
+        <f t="shared" si="6"/>
+        <v>9.6000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="109" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D109" s="79" t="s">
+        <v>93</v>
+      </c>
+      <c r="E109" s="80">
+        <f>0.00005</f>
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="F109" s="80">
+        <f t="shared" si="6"/>
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D110" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="E110" s="80">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="F110" s="80">
+        <f t="shared" si="6"/>
+        <v>5.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D111" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="E111" s="80"/>
+      <c r="F111" s="80">
+        <f t="shared" si="6"/>
+        <v>5.7099999999999998E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D112" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="E112" s="80"/>
+      <c r="F112" s="78"/>
+    </row>
+    <row r="113" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="C113" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D113" s="71"/>
+      <c r="E113" s="80"/>
+      <c r="F113" s="78"/>
+    </row>
+    <row r="114" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D114" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="E114" s="80">
+        <v>0.25609999999999999</v>
+      </c>
+      <c r="F114" s="78"/>
+    </row>
+    <row r="115" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D115" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="E115" s="80">
+        <v>2.877E-2</v>
+      </c>
+      <c r="F115" s="78"/>
+    </row>
+    <row r="116" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D116" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="E116" s="80">
+        <v>3.1220000000000001E-2</v>
+      </c>
+      <c r="F116" s="78"/>
+    </row>
+    <row r="117" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D117" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="E117" s="80">
+        <v>3.109E-2</v>
+      </c>
+      <c r="F117" s="78"/>
+    </row>
+    <row r="118" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D118" s="79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E118" s="80">
+        <v>3.3250000000000002E-2</v>
+      </c>
+      <c r="F118" s="78"/>
+    </row>
+    <row r="119" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D119" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="E119" s="80">
+        <v>3.372E-2</v>
+      </c>
+      <c r="F119" s="78"/>
+    </row>
+    <row r="120" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D120" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="E120" s="80">
+        <v>3.354E-2</v>
+      </c>
+      <c r="F120" s="78"/>
+    </row>
+    <row r="121" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D121" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="E121" s="80">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="F121" s="78"/>
+    </row>
+    <row r="122" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D122" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="E122" s="80">
+        <v>3.3340000000000002E-2</v>
+      </c>
+      <c r="F122" s="78"/>
+    </row>
+    <row r="123" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D123" s="79" t="s">
+        <v>105</v>
+      </c>
+      <c r="E123" s="80">
+        <v>3.3360000000000001E-2</v>
+      </c>
+      <c r="F123" s="78"/>
+    </row>
+    <row r="124" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D124" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E124" s="80">
+        <v>3.5549999999999998E-2</v>
+      </c>
+      <c r="F124" s="78"/>
+    </row>
+    <row r="125" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D125" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="E125" s="1">
+        <v>4.2430000000000002E-2</v>
+      </c>
+      <c r="F125" s="1"/>
+    </row>
+    <row r="126" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D126" s="79"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127" spans="3:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="D127" s="76" t="s">
+        <v>85</v>
+      </c>
+      <c r="E127" s="77"/>
+      <c r="F127" s="78"/>
+    </row>
+    <row r="129" spans="3:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="C129" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="D129" s="81"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D130" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="E130" s="80">
+        <v>-3.7780000000000001E-2</v>
+      </c>
+      <c r="F130" s="6">
+        <f>$E$92+E130</f>
+        <v>0.24429999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D131" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E131" s="80">
+        <v>2.5350000000000001E-2</v>
+      </c>
+      <c r="F131" s="6">
+        <f t="shared" ref="F131:F132" si="7">$E$92+E131</f>
+        <v>0.30742999999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="3:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="D132" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E132" s="80">
+        <v>0.1022</v>
+      </c>
+      <c r="F132" s="6">
+        <f t="shared" si="7"/>
+        <v>0.38428000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C113:D113"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="G57:H57"/>
@@ -3049,6 +3629,7 @@
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="H19:K19"/>
   </mergeCells>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>